<commit_message>
Forgot to add Michigan earlier
</commit_message>
<xml_diff>
--- a/Finished States/Michigan (OSB).xlsx
+++ b/Finished States/Michigan (OSB).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caseyrand/Documents/Github/sports-betting/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caseyrand/Documents/Github/sports-betting/Finished States/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50BCC028-EAC3-254A-BC98-1CB05BA9699A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B6C07E-7D9C-A642-8020-F2DCA315D943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -217,7 +217,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -274,7 +274,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -581,7 +581,8 @@
   <dimension ref="A1:K579"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <pane ySplit="1" topLeftCell="A557" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D576" sqref="D576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>